<commit_message>
STYLE: update code for geom optimizations
</commit_message>
<xml_diff>
--- a/Data/extracts/o-series.xlsx
+++ b/Data/extracts/o-series.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:S36"/>
+  <dimension ref="B3:S60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +531,7 @@
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>def2svpd</t>
+          <t>pcX-2</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -540,19 +540,17 @@
         </is>
       </c>
       <c r="F4" s="1" t="n">
-        <v>541.307815</v>
+        <v>538.860887</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>542.388459</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>542.294585</v>
-      </c>
+        <v>539.953355</v>
+      </c>
+      <c r="H4" s="1" t="n"/>
       <c r="I4" s="1" t="n">
-        <v>542.324226</v>
+        <v>539.994237</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>542.374131</v>
+        <v>540.045514</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>539.9</v>
@@ -568,13 +566,13 @@
         </is>
       </c>
       <c r="N4" s="1" t="n">
-        <v>0.0112</v>
+        <v>0.0063</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>0.0107</v>
+        <v>0.0081</v>
       </c>
       <c r="P4" s="1" t="n">
-        <v>0.0148</v>
+        <v>0.0119</v>
       </c>
       <c r="Q4" s="1" t="n"/>
       <c r="R4" s="1" t="n"/>
@@ -593,7 +591,7 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>3-21G</t>
+          <t>def2svpd</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
@@ -602,19 +600,19 @@
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>538.617</v>
+        <v>541.307815</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>538.791459</v>
+        <v>542.388459</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>538.833151</v>
+        <v>542.294585</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>538.844834</v>
+        <v>542.324226</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>538.861479</v>
+        <v>542.374131</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>539.9</v>
@@ -630,13 +628,13 @@
         </is>
       </c>
       <c r="N5" s="1" t="n">
-        <v>0.0055</v>
+        <v>0.0112</v>
       </c>
       <c r="O5" s="1" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.0107</v>
       </c>
       <c r="P5" s="1" t="n">
-        <v>0.0122</v>
+        <v>0.0148</v>
       </c>
       <c r="Q5" s="1" t="n"/>
       <c r="R5" s="1" t="n"/>
@@ -655,7 +653,7 @@
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>STO-6G</t>
+          <t>pcX-4</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
@@ -664,20 +662,14 @@
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>548.685289</v>
+        <v>538.8684009999999</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>549.199239</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>549.36981</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>549.44602</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>549.4434220000001</v>
-      </c>
+        <v>539.9276159999999</v>
+      </c>
+      <c r="H6" s="1" t="n"/>
+      <c r="I6" s="1" t="n"/>
+      <c r="J6" s="1" t="n"/>
       <c r="K6" s="1" t="n">
         <v>539.9</v>
       </c>
@@ -691,15 +683,9 @@
           <t xml:space="preserve"> [[[0, 4]], []]</t>
         </is>
       </c>
-      <c r="N6" s="1" t="n">
-        <v>0.0044</v>
-      </c>
-      <c r="O6" s="1" t="n">
-        <v>0.007900000000000001</v>
-      </c>
-      <c r="P6" s="1" t="n">
-        <v>0.008399999999999999</v>
-      </c>
+      <c r="N6" s="1" t="n"/>
+      <c r="O6" s="1" t="n"/>
+      <c r="P6" s="1" t="n"/>
       <c r="Q6" s="1" t="n"/>
       <c r="R6" s="1" t="n"/>
       <c r="S6" s="1" t="n"/>
@@ -717,7 +703,7 @@
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>pcX-3</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
@@ -726,19 +712,17 @@
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>538.931335</v>
+        <v>538.868505</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>540.005054</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>540.060415</v>
-      </c>
+        <v>539.926299</v>
+      </c>
+      <c r="H7" s="1" t="n"/>
       <c r="I7" s="1" t="n">
-        <v>540.054773</v>
+        <v>539.943388</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>540.103879</v>
+        <v>540.007018</v>
       </c>
       <c r="K7" s="1" t="n">
         <v>539.9</v>
@@ -754,13 +738,13 @@
         </is>
       </c>
       <c r="N7" s="1" t="n">
-        <v>0.0059</v>
+        <v>0.008</v>
       </c>
       <c r="O7" s="1" t="n">
-        <v>0.008</v>
+        <v>0.008200000000000001</v>
       </c>
       <c r="P7" s="1" t="n">
-        <v>0.0117</v>
+        <v>0.011</v>
       </c>
       <c r="Q7" s="1" t="n"/>
       <c r="R7" s="1" t="n"/>
@@ -779,7 +763,7 @@
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>4-31G</t>
+          <t>3-21G</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr">
@@ -788,19 +772,19 @@
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>540.573025</v>
+        <v>538.617</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>541.383392</v>
+        <v>538.791459</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>541.362338</v>
+        <v>538.833151</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>541.394864</v>
+        <v>538.844834</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>541.38633</v>
+        <v>538.861479</v>
       </c>
       <c r="K8" s="1" t="n">
         <v>539.9</v>
@@ -816,13 +800,13 @@
         </is>
       </c>
       <c r="N8" s="1" t="n">
-        <v>0.0058</v>
+        <v>0.0055</v>
       </c>
       <c r="O8" s="1" t="n">
-        <v>0.0098</v>
+        <v>0.008200000000000001</v>
       </c>
       <c r="P8" s="1" t="n">
-        <v>0.0144</v>
+        <v>0.0122</v>
       </c>
       <c r="Q8" s="1" t="n"/>
       <c r="R8" s="1" t="n"/>
@@ -841,7 +825,7 @@
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>6-31G</t>
+          <t>STO-6G</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
@@ -850,19 +834,19 @@
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>541.735471</v>
+        <v>548.685289</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>542.655761</v>
+        <v>549.199239</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>542.625577</v>
+        <v>549.36981</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>542.662198</v>
+        <v>549.44602</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>542.65022</v>
+        <v>549.4434220000001</v>
       </c>
       <c r="K9" s="1" t="n">
         <v>539.9</v>
@@ -878,13 +862,13 @@
         </is>
       </c>
       <c r="N9" s="1" t="n">
-        <v>0.006</v>
+        <v>0.0044</v>
       </c>
       <c r="O9" s="1" t="n">
-        <v>0.0103</v>
+        <v>0.007900000000000001</v>
       </c>
       <c r="P9" s="1" t="n">
-        <v>0.0146</v>
+        <v>0.008399999999999999</v>
       </c>
       <c r="Q9" s="1" t="n"/>
       <c r="R9" s="1" t="n"/>
@@ -903,7 +887,7 @@
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>def2svp</t>
+          <t>ccX-TZ</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr">
@@ -912,19 +896,17 @@
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>541.0810269999999</v>
+        <v>538.86105</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>541.912914</v>
-      </c>
-      <c r="H10" s="1" t="n">
-        <v>541.876919</v>
-      </c>
+        <v>540.044391</v>
+      </c>
+      <c r="H10" s="1" t="n"/>
       <c r="I10" s="1" t="n">
-        <v>541.8921790000001</v>
+        <v>540.07417</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>541.902976</v>
+        <v>540.1306949999999</v>
       </c>
       <c r="K10" s="1" t="n">
         <v>539.9</v>
@@ -940,13 +922,13 @@
         </is>
       </c>
       <c r="N10" s="1" t="n">
-        <v>0.0053</v>
+        <v>0.008</v>
       </c>
       <c r="O10" s="1" t="n">
-        <v>0.0083</v>
+        <v>0.008399999999999999</v>
       </c>
       <c r="P10" s="1" t="n">
-        <v>0.0135</v>
+        <v>0.0116</v>
       </c>
       <c r="Q10" s="1" t="n"/>
       <c r="R10" s="1" t="n"/>
@@ -965,7 +947,7 @@
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>STO-3G</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr">
@@ -974,19 +956,19 @@
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>541.681967</v>
+        <v>538.931335</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>542.18669</v>
+        <v>540.005054</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>542.353803</v>
+        <v>540.060415</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>542.428404</v>
+        <v>540.054773</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>542.425909</v>
+        <v>540.103879</v>
       </c>
       <c r="K11" s="1" t="n">
         <v>539.9</v>
@@ -1002,13 +984,13 @@
         </is>
       </c>
       <c r="N11" s="1" t="n">
-        <v>0.0043</v>
+        <v>0.0059</v>
       </c>
       <c r="O11" s="1" t="n">
-        <v>0.0078</v>
+        <v>0.008</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.0117</v>
       </c>
       <c r="Q11" s="1" t="n"/>
       <c r="R11" s="1" t="n"/>
@@ -1027,7 +1009,7 @@
       </c>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>ccX-5Z</t>
         </is>
       </c>
       <c r="E12" s="1" t="inlineStr">
@@ -1036,20 +1018,14 @@
         </is>
       </c>
       <c r="F12" s="1" t="n">
-        <v>540.039626</v>
+        <v>538.867026</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>541.587282</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>541.609076</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>541.621315</v>
-      </c>
-      <c r="J12" s="1" t="n">
-        <v>541.635627</v>
-      </c>
+        <v>539.979908</v>
+      </c>
+      <c r="H12" s="1" t="n"/>
+      <c r="I12" s="1" t="n"/>
+      <c r="J12" s="1" t="n"/>
       <c r="K12" s="1" t="n">
         <v>539.9</v>
       </c>
@@ -1063,15 +1039,9 @@
           <t xml:space="preserve"> [[[0, 4]], []]</t>
         </is>
       </c>
-      <c r="N12" s="1" t="n">
-        <v>0.0053</v>
-      </c>
-      <c r="O12" s="1" t="n">
-        <v>0.0081</v>
-      </c>
-      <c r="P12" s="1" t="n">
-        <v>0.0134</v>
-      </c>
+      <c r="N12" s="1" t="n"/>
+      <c r="O12" s="1" t="n"/>
+      <c r="P12" s="1" t="n"/>
       <c r="Q12" s="1" t="n"/>
       <c r="R12" s="1" t="n"/>
       <c r="S12" s="1" t="n"/>
@@ -1089,7 +1059,7 @@
       </c>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>pcX-1</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr">
@@ -1098,19 +1068,17 @@
         </is>
       </c>
       <c r="F13" s="1" t="n">
-        <v>538.868235</v>
+        <v>538.903363</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>539.962179</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>539.988344</v>
-      </c>
+        <v>539.8414770000001</v>
+      </c>
+      <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n">
-        <v>539.9867850000001</v>
+        <v>539.965946</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>540.04421</v>
+        <v>539.974185</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>539.9</v>
@@ -1126,13 +1094,13 @@
         </is>
       </c>
       <c r="N13" s="1" t="n">
-        <v>0.0066</v>
+        <v>0.0047</v>
       </c>
       <c r="O13" s="1" t="n">
-        <v>0.0083</v>
+        <v>0.0071</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>0.0109</v>
+        <v>0.0123</v>
       </c>
       <c r="Q13" s="1" t="n"/>
       <c r="R13" s="1" t="n"/>
@@ -1151,7 +1119,7 @@
       </c>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4-31G</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr">
@@ -1160,14 +1128,20 @@
         </is>
       </c>
       <c r="F14" s="1" t="n">
-        <v>538.864346</v>
+        <v>540.573025</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>539.963262</v>
-      </c>
-      <c r="H14" s="1" t="n"/>
-      <c r="I14" s="1" t="n"/>
-      <c r="J14" s="1" t="n"/>
+        <v>541.383392</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>541.362338</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>541.394864</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>541.38633</v>
+      </c>
       <c r="K14" s="1" t="n">
         <v>539.9</v>
       </c>
@@ -1181,9 +1155,15 @@
           <t xml:space="preserve"> [[[0, 4]], []]</t>
         </is>
       </c>
-      <c r="N14" s="1" t="n"/>
-      <c r="O14" s="1" t="n"/>
-      <c r="P14" s="1" t="n"/>
+      <c r="N14" s="1" t="n">
+        <v>0.0058</v>
+      </c>
+      <c r="O14" s="1" t="n">
+        <v>0.0098</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>0.0144</v>
+      </c>
       <c r="Q14" s="1" t="n"/>
       <c r="R14" s="1" t="n"/>
       <c r="S14" s="1" t="n"/>
@@ -1191,7 +1171,7 @@
     <row r="15">
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>h2o</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
@@ -1201,7 +1181,7 @@
       </c>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>def2svpd</t>
+          <t>6-31G</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr">
@@ -1210,41 +1190,41 @@
         </is>
       </c>
       <c r="F15" s="1" t="n">
-        <v>543.717543</v>
+        <v>541.735471</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>545.322461</v>
+        <v>542.655761</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>544.958337</v>
+        <v>542.625577</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>544.912727</v>
+        <v>542.662198</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>545.008721</v>
+        <v>542.65022</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>542.55</v>
+        <v>539.9</v>
       </c>
       <c r="L15" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[6], []]</t>
+          <t xml:space="preserve"> [[4], []]</t>
         </is>
       </c>
       <c r="M15" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 6]], []]</t>
+          <t xml:space="preserve"> [[[0, 4]], []]</t>
         </is>
       </c>
       <c r="N15" s="1" t="n">
-        <v>0.0166</v>
+        <v>0.006</v>
       </c>
       <c r="O15" s="1" t="n">
-        <v>0.0232</v>
+        <v>0.0103</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.0268</v>
+        <v>0.0146</v>
       </c>
       <c r="Q15" s="1" t="n"/>
       <c r="R15" s="1" t="n"/>
@@ -1253,7 +1233,7 @@
     <row r="16">
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>h2o</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
@@ -1263,7 +1243,7 @@
       </c>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>3-21G</t>
+          <t>ccX-DZ</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr">
@@ -1272,41 +1252,39 @@
         </is>
       </c>
       <c r="F16" s="1" t="n">
-        <v>541.775266</v>
+        <v>538.880872</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>542.81729</v>
-      </c>
-      <c r="H16" s="1" t="n">
-        <v>542.460297</v>
-      </c>
+        <v>540.063637</v>
+      </c>
+      <c r="H16" s="1" t="n"/>
       <c r="I16" s="1" t="n">
-        <v>542.42638</v>
+        <v>540.136292</v>
       </c>
       <c r="J16" s="1" t="n">
-        <v>542.492736</v>
+        <v>540.178217</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>542.55</v>
+        <v>539.9</v>
       </c>
       <c r="L16" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[6], []]</t>
+          <t xml:space="preserve"> [[4], []]</t>
         </is>
       </c>
       <c r="M16" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 6]], []]</t>
+          <t xml:space="preserve"> [[[0, 4]], []]</t>
         </is>
       </c>
       <c r="N16" s="1" t="n">
-        <v>0.017</v>
+        <v>0.0083</v>
       </c>
       <c r="O16" s="1" t="n">
-        <v>0.0245</v>
+        <v>0.008800000000000001</v>
       </c>
       <c r="P16" s="1" t="n">
-        <v>0.0274</v>
+        <v>0.0127</v>
       </c>
       <c r="Q16" s="1" t="n"/>
       <c r="R16" s="1" t="n"/>
@@ -1315,7 +1293,7 @@
     <row r="17">
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>h2o</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
@@ -1325,7 +1303,7 @@
       </c>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>STO-6G</t>
+          <t>def2svp</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr">
@@ -1334,41 +1312,41 @@
         </is>
       </c>
       <c r="F17" s="1" t="n">
-        <v>553.093948</v>
+        <v>541.0810269999999</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>555.006122</v>
+        <v>541.912914</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>554.653621</v>
+        <v>541.876919</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>554.575449</v>
+        <v>541.8921790000001</v>
       </c>
       <c r="J17" s="1" t="n">
-        <v>554.650545</v>
+        <v>541.902976</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>542.55</v>
+        <v>539.9</v>
       </c>
       <c r="L17" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[6], []]</t>
+          <t xml:space="preserve"> [[4], []]</t>
         </is>
       </c>
       <c r="M17" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 6]], []]</t>
+          <t xml:space="preserve"> [[[0, 4]], []]</t>
         </is>
       </c>
       <c r="N17" s="1" t="n">
-        <v>0.0179</v>
+        <v>0.0053</v>
       </c>
       <c r="O17" s="1" t="n">
-        <v>0.0209</v>
+        <v>0.0083</v>
       </c>
       <c r="P17" s="1" t="n">
-        <v>0.0196</v>
+        <v>0.0135</v>
       </c>
       <c r="Q17" s="1" t="n"/>
       <c r="R17" s="1" t="n"/>
@@ -1377,7 +1355,7 @@
     <row r="18">
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>h2o</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
@@ -1387,7 +1365,7 @@
       </c>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>STO-3G</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr">
@@ -1396,41 +1374,41 @@
         </is>
       </c>
       <c r="F18" s="1" t="n">
-        <v>541.331326</v>
+        <v>541.681967</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>543.012565</v>
+        <v>542.18669</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>542.7990600000001</v>
+        <v>542.353803</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>542.73607</v>
+        <v>542.428404</v>
       </c>
       <c r="J18" s="1" t="n">
-        <v>542.851467</v>
+        <v>542.425909</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>542.55</v>
+        <v>539.9</v>
       </c>
       <c r="L18" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[6], []]</t>
+          <t xml:space="preserve"> [[4], []]</t>
         </is>
       </c>
       <c r="M18" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 6]], []]</t>
+          <t xml:space="preserve"> [[[0, 4]], []]</t>
         </is>
       </c>
       <c r="N18" s="1" t="n">
-        <v>0.0154</v>
+        <v>0.0043</v>
       </c>
       <c r="O18" s="1" t="n">
-        <v>0.0198</v>
+        <v>0.0078</v>
       </c>
       <c r="P18" s="1" t="n">
-        <v>0.0251</v>
+        <v>0.008200000000000001</v>
       </c>
       <c r="Q18" s="1" t="n"/>
       <c r="R18" s="1" t="n"/>
@@ -1439,7 +1417,7 @@
     <row r="19">
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>h2o</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
@@ -1449,7 +1427,7 @@
       </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>4-31G</t>
+          <t>ccX-QZ</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr">
@@ -1458,41 +1436,39 @@
         </is>
       </c>
       <c r="F19" s="1" t="n">
-        <v>543.367484</v>
+        <v>538.865032</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>544.966489</v>
-      </c>
-      <c r="H19" s="1" t="n">
-        <v>544.528882</v>
-      </c>
+        <v>540.000039</v>
+      </c>
+      <c r="H19" s="1" t="n"/>
       <c r="I19" s="1" t="n">
-        <v>544.518913</v>
+        <v>540.013434</v>
       </c>
       <c r="J19" s="1" t="n">
-        <v>544.550709</v>
+        <v>540.074888</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>542.55</v>
+        <v>539.9</v>
       </c>
       <c r="L19" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[6], []]</t>
+          <t xml:space="preserve"> [[4], []]</t>
         </is>
       </c>
       <c r="M19" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 6]], []]</t>
+          <t xml:space="preserve"> [[[0, 4]], []]</t>
         </is>
       </c>
       <c r="N19" s="1" t="n">
-        <v>0.0177</v>
+        <v>0.0078</v>
       </c>
       <c r="O19" s="1" t="n">
-        <v>0.0258</v>
+        <v>0.008399999999999999</v>
       </c>
       <c r="P19" s="1" t="n">
-        <v>0.0287</v>
+        <v>0.0108</v>
       </c>
       <c r="Q19" s="1" t="n"/>
       <c r="R19" s="1" t="n"/>
@@ -1501,7 +1477,7 @@
     <row r="20">
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>h2o</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
@@ -1511,7 +1487,7 @@
       </c>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>6-31G</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr">
@@ -1520,41 +1496,41 @@
         </is>
       </c>
       <c r="F20" s="1" t="n">
-        <v>544.538315</v>
+        <v>540.039626</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>546.241719</v>
+        <v>541.587282</v>
       </c>
       <c r="H20" s="1" t="n">
-        <v>545.79014</v>
+        <v>541.609076</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>545.786166</v>
+        <v>541.621315</v>
       </c>
       <c r="J20" s="1" t="n">
-        <v>545.811799</v>
+        <v>541.635627</v>
       </c>
       <c r="K20" s="1" t="n">
-        <v>542.55</v>
+        <v>539.9</v>
       </c>
       <c r="L20" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[6], []]</t>
+          <t xml:space="preserve"> [[4], []]</t>
         </is>
       </c>
       <c r="M20" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 6]], []]</t>
+          <t xml:space="preserve"> [[[0, 4]], []]</t>
         </is>
       </c>
       <c r="N20" s="1" t="n">
-        <v>0.0179</v>
+        <v>0.0053</v>
       </c>
       <c r="O20" s="1" t="n">
-        <v>0.026</v>
+        <v>0.0081</v>
       </c>
       <c r="P20" s="1" t="n">
-        <v>0.0286</v>
+        <v>0.0134</v>
       </c>
       <c r="Q20" s="1" t="n"/>
       <c r="R20" s="1" t="n"/>
@@ -1563,7 +1539,7 @@
     <row r="21">
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>h2o</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
@@ -1573,7 +1549,7 @@
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>def2svp</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr">
@@ -1582,41 +1558,41 @@
         </is>
       </c>
       <c r="F21" s="1" t="n">
-        <v>543.682769</v>
+        <v>538.868235</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>545.204682</v>
+        <v>539.962179</v>
       </c>
       <c r="H21" s="1" t="n">
-        <v>544.834432</v>
+        <v>539.988344</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>544.798126</v>
+        <v>539.9867850000001</v>
       </c>
       <c r="J21" s="1" t="n">
-        <v>544.868799</v>
+        <v>540.04421</v>
       </c>
       <c r="K21" s="1" t="n">
-        <v>542.55</v>
+        <v>539.9</v>
       </c>
       <c r="L21" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[6], []]</t>
+          <t xml:space="preserve"> [[4], []]</t>
         </is>
       </c>
       <c r="M21" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 6]], []]</t>
+          <t xml:space="preserve"> [[[0, 4]], []]</t>
         </is>
       </c>
       <c r="N21" s="1" t="n">
-        <v>0.0167</v>
+        <v>0.0066</v>
       </c>
       <c r="O21" s="1" t="n">
-        <v>0.0234</v>
+        <v>0.0083</v>
       </c>
       <c r="P21" s="1" t="n">
-        <v>0.0268</v>
+        <v>0.0109</v>
       </c>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
@@ -1625,7 +1601,7 @@
     <row r="22">
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>h2o</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
@@ -1635,7 +1611,7 @@
       </c>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>STO-3G</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr">
@@ -1644,42 +1620,30 @@
         </is>
       </c>
       <c r="F22" s="1" t="n">
-        <v>546.120439</v>
+        <v>538.864346</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>548.022062</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <v>547.674501</v>
-      </c>
-      <c r="I22" s="1" t="n">
-        <v>547.5980070000001</v>
-      </c>
-      <c r="J22" s="1" t="n">
-        <v>547.669324</v>
-      </c>
+        <v>539.963262</v>
+      </c>
+      <c r="H22" s="1" t="n"/>
+      <c r="I22" s="1" t="n"/>
+      <c r="J22" s="1" t="n"/>
       <c r="K22" s="1" t="n">
-        <v>542.55</v>
+        <v>539.9</v>
       </c>
       <c r="L22" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[6], []]</t>
+          <t xml:space="preserve"> [[4], []]</t>
         </is>
       </c>
       <c r="M22" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 6]], []]</t>
-        </is>
-      </c>
-      <c r="N22" s="1" t="n">
-        <v>0.0176</v>
-      </c>
-      <c r="O22" s="1" t="n">
-        <v>0.0207</v>
-      </c>
-      <c r="P22" s="1" t="n">
-        <v>0.0194</v>
-      </c>
+          <t xml:space="preserve"> [[[0, 4]], []]</t>
+        </is>
+      </c>
+      <c r="N22" s="1" t="n"/>
+      <c r="O22" s="1" t="n"/>
+      <c r="P22" s="1" t="n"/>
       <c r="Q22" s="1" t="n"/>
       <c r="R22" s="1" t="n"/>
       <c r="S22" s="1" t="n"/>
@@ -1697,7 +1661,7 @@
       </c>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>pcX-2</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr">
@@ -1706,19 +1670,17 @@
         </is>
       </c>
       <c r="F23" s="1" t="n">
-        <v>542.589644</v>
+        <v>541.194543</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>544.813564</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <v>544.527342</v>
-      </c>
+        <v>542.862973</v>
+      </c>
+      <c r="H23" s="1" t="n"/>
       <c r="I23" s="1" t="n">
-        <v>544.4855209999999</v>
+        <v>542.591932</v>
       </c>
       <c r="J23" s="1" t="n">
-        <v>544.557104</v>
+        <v>542.704069</v>
       </c>
       <c r="K23" s="1" t="n">
         <v>542.55</v>
@@ -1734,13 +1696,13 @@
         </is>
       </c>
       <c r="N23" s="1" t="n">
-        <v>0.0162</v>
+        <v>0.0155</v>
       </c>
       <c r="O23" s="1" t="n">
-        <v>0.023</v>
+        <v>0.0198</v>
       </c>
       <c r="P23" s="1" t="n">
-        <v>0.0267</v>
+        <v>0.0249</v>
       </c>
       <c r="Q23" s="1" t="n"/>
       <c r="R23" s="1" t="n"/>
@@ -1759,7 +1721,7 @@
       </c>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>def2svpd</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr">
@@ -1768,19 +1730,19 @@
         </is>
       </c>
       <c r="F24" s="1" t="n">
-        <v>541.207688</v>
+        <v>543.717543</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>542.90394</v>
+        <v>545.322461</v>
       </c>
       <c r="H24" s="1" t="n">
-        <v>542.675713</v>
+        <v>544.958337</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>542.612129</v>
+        <v>544.912727</v>
       </c>
       <c r="J24" s="1" t="n">
-        <v>542.7326880000001</v>
+        <v>545.008721</v>
       </c>
       <c r="K24" s="1" t="n">
         <v>542.55</v>
@@ -1796,13 +1758,13 @@
         </is>
       </c>
       <c r="N24" s="1" t="n">
-        <v>0.0152</v>
+        <v>0.0166</v>
       </c>
       <c r="O24" s="1" t="n">
-        <v>0.0192</v>
+        <v>0.0232</v>
       </c>
       <c r="P24" s="1" t="n">
-        <v>0.0246</v>
+        <v>0.0268</v>
       </c>
       <c r="Q24" s="1" t="n"/>
       <c r="R24" s="1" t="n"/>
@@ -1821,7 +1783,7 @@
       </c>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>pcX-4</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr">
@@ -1830,10 +1792,10 @@
         </is>
       </c>
       <c r="F25" s="1" t="n">
-        <v>541.181632</v>
+        <v>541.180401</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>542.878792</v>
+        <v>542.83172</v>
       </c>
       <c r="H25" s="1" t="n"/>
       <c r="I25" s="1" t="n"/>
@@ -1861,7 +1823,7 @@
     <row r="26">
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>co2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr">
@@ -1871,7 +1833,7 @@
       </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>def2svpd</t>
+          <t>pcX-3</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr">
@@ -1880,41 +1842,39 @@
         </is>
       </c>
       <c r="F26" s="1" t="n">
-        <v>542.840658</v>
+        <v>541.182672</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>543.7178730000001</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>543.622133</v>
-      </c>
+        <v>542.822688</v>
+      </c>
+      <c r="H26" s="1" t="n"/>
       <c r="I26" s="1" t="n">
-        <v>543.587229</v>
+        <v>542.5327590000001</v>
       </c>
       <c r="J26" s="1" t="n">
-        <v>543.64082</v>
+        <v>542.654593</v>
       </c>
       <c r="K26" s="1" t="n">
-        <v>541.34</v>
+        <v>542.55</v>
       </c>
       <c r="L26" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[10], []]</t>
+          <t xml:space="preserve"> [[6], []]</t>
         </is>
       </c>
       <c r="M26" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 10]], []]</t>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
         </is>
       </c>
       <c r="N26" s="1" t="n">
-        <v>0.0162</v>
+        <v>0.0153</v>
       </c>
       <c r="O26" s="1" t="n">
-        <v>0.0272</v>
+        <v>0.0195</v>
       </c>
       <c r="P26" s="1" t="n">
-        <v>0.0218</v>
+        <v>0.0248</v>
       </c>
       <c r="Q26" s="1" t="n"/>
       <c r="R26" s="1" t="n"/>
@@ -1923,7 +1883,7 @@
     <row r="27">
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>co2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
@@ -1942,41 +1902,41 @@
         </is>
       </c>
       <c r="F27" s="1" t="n">
-        <v>540.712431</v>
+        <v>541.775266</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>540.817708</v>
+        <v>542.81729</v>
       </c>
       <c r="H27" s="1" t="n">
-        <v>540.803845</v>
+        <v>542.460297</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>540.76192</v>
+        <v>542.42638</v>
       </c>
       <c r="J27" s="1" t="n">
-        <v>540.820592</v>
+        <v>542.492736</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>541.34</v>
+        <v>542.55</v>
       </c>
       <c r="L27" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[10], []]</t>
+          <t xml:space="preserve"> [[6], []]</t>
         </is>
       </c>
       <c r="M27" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 10]], []]</t>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
         </is>
       </c>
       <c r="N27" s="1" t="n">
-        <v>0.0173</v>
+        <v>0.017</v>
       </c>
       <c r="O27" s="1" t="n">
-        <v>0.0303</v>
+        <v>0.0245</v>
       </c>
       <c r="P27" s="1" t="n">
-        <v>0.0201</v>
+        <v>0.0274</v>
       </c>
       <c r="Q27" s="1" t="n"/>
       <c r="R27" s="1" t="n"/>
@@ -1985,7 +1945,7 @@
     <row r="28">
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>co2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr">
@@ -2004,41 +1964,41 @@
         </is>
       </c>
       <c r="F28" s="1" t="n">
-        <v>550.647015</v>
+        <v>553.093948</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>551.428781</v>
+        <v>555.006122</v>
       </c>
       <c r="H28" s="1" t="n">
-        <v>551.142123</v>
+        <v>554.653621</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>551.1091300000001</v>
+        <v>554.575449</v>
       </c>
       <c r="J28" s="1" t="n">
-        <v>551.429568</v>
+        <v>554.650545</v>
       </c>
       <c r="K28" s="1" t="n">
-        <v>541.34</v>
+        <v>542.55</v>
       </c>
       <c r="L28" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[10], []]</t>
+          <t xml:space="preserve"> [[6], []]</t>
         </is>
       </c>
       <c r="M28" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 10]], []]</t>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
         </is>
       </c>
       <c r="N28" s="1" t="n">
-        <v>0.0187</v>
+        <v>0.0179</v>
       </c>
       <c r="O28" s="1" t="n">
-        <v>0.0417</v>
+        <v>0.0209</v>
       </c>
       <c r="P28" s="1" t="n">
-        <v>0.0103</v>
+        <v>0.0196</v>
       </c>
       <c r="Q28" s="1" t="n"/>
       <c r="R28" s="1" t="n"/>
@@ -2047,7 +2007,7 @@
     <row r="29">
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>co2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr">
@@ -2057,7 +2017,7 @@
       </c>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>ccX-TZ</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr">
@@ -2066,41 +2026,39 @@
         </is>
       </c>
       <c r="F29" s="1" t="n">
-        <v>540.50555</v>
+        <v>541.1865780000001</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>541.48218</v>
-      </c>
-      <c r="H29" s="1" t="n">
-        <v>541.539387</v>
-      </c>
+        <v>542.9247329999999</v>
+      </c>
+      <c r="H29" s="1" t="n"/>
       <c r="I29" s="1" t="n">
-        <v>541.475468</v>
+        <v>542.649096</v>
       </c>
       <c r="J29" s="1" t="n">
-        <v>541.526035</v>
+        <v>542.763499</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>541.34</v>
+        <v>542.55</v>
       </c>
       <c r="L29" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[10], []]</t>
+          <t xml:space="preserve"> [[6], []]</t>
         </is>
       </c>
       <c r="M29" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 10]], []]</t>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
         </is>
       </c>
       <c r="N29" s="1" t="n">
         <v>0.0154</v>
       </c>
       <c r="O29" s="1" t="n">
-        <v>0.0262</v>
+        <v>0.0196</v>
       </c>
       <c r="P29" s="1" t="n">
-        <v>0.0206</v>
+        <v>0.0249</v>
       </c>
       <c r="Q29" s="1" t="n"/>
       <c r="R29" s="1" t="n"/>
@@ -2109,7 +2067,7 @@
     <row r="30">
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>co2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr">
@@ -2119,7 +2077,7 @@
       </c>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>4-31G</t>
+          <t>T</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr">
@@ -2128,41 +2086,41 @@
         </is>
       </c>
       <c r="F30" s="1" t="n">
-        <v>542.634949</v>
+        <v>541.331326</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>543.299207</v>
+        <v>543.012565</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>543.241</v>
+        <v>542.7990600000001</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>543.20036</v>
+        <v>542.73607</v>
       </c>
       <c r="J30" s="1" t="n">
-        <v>543.227394</v>
+        <v>542.851467</v>
       </c>
       <c r="K30" s="1" t="n">
-        <v>541.34</v>
+        <v>542.55</v>
       </c>
       <c r="L30" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[10], []]</t>
+          <t xml:space="preserve"> [[6], []]</t>
         </is>
       </c>
       <c r="M30" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 10]], []]</t>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
         </is>
       </c>
       <c r="N30" s="1" t="n">
-        <v>0.0172</v>
+        <v>0.0154</v>
       </c>
       <c r="O30" s="1" t="n">
-        <v>0.0326</v>
+        <v>0.0198</v>
       </c>
       <c r="P30" s="1" t="n">
-        <v>0.0206</v>
+        <v>0.0251</v>
       </c>
       <c r="Q30" s="1" t="n"/>
       <c r="R30" s="1" t="n"/>
@@ -2171,7 +2129,7 @@
     <row r="31">
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>co2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
@@ -2181,7 +2139,7 @@
       </c>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>6-31G</t>
+          <t>ccX-5Z</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr">
@@ -2190,42 +2148,30 @@
         </is>
       </c>
       <c r="F31" s="1" t="n">
-        <v>543.774725</v>
+        <v>541.179586</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>544.53587</v>
-      </c>
-      <c r="H31" s="1" t="n">
-        <v>544.465741</v>
-      </c>
-      <c r="I31" s="1" t="n">
-        <v>544.4301390000001</v>
-      </c>
-      <c r="J31" s="1" t="n">
-        <v>544.45589</v>
-      </c>
+        <v>542.885472</v>
+      </c>
+      <c r="H31" s="1" t="n"/>
+      <c r="I31" s="1" t="n"/>
+      <c r="J31" s="1" t="n"/>
       <c r="K31" s="1" t="n">
-        <v>541.34</v>
+        <v>542.55</v>
       </c>
       <c r="L31" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[10], []]</t>
+          <t xml:space="preserve"> [[6], []]</t>
         </is>
       </c>
       <c r="M31" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 10]], []]</t>
-        </is>
-      </c>
-      <c r="N31" s="1" t="n">
-        <v>0.0171</v>
-      </c>
-      <c r="O31" s="1" t="n">
-        <v>0.0325</v>
-      </c>
-      <c r="P31" s="1" t="n">
-        <v>0.0205</v>
-      </c>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
+        </is>
+      </c>
+      <c r="N31" s="1" t="n"/>
+      <c r="O31" s="1" t="n"/>
+      <c r="P31" s="1" t="n"/>
       <c r="Q31" s="1" t="n"/>
       <c r="R31" s="1" t="n"/>
       <c r="S31" s="1" t="n"/>
@@ -2233,7 +2179,7 @@
     <row r="32">
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>co2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr">
@@ -2243,7 +2189,7 @@
       </c>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>def2svp</t>
+          <t>pcX-1</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr">
@@ -2252,41 +2198,39 @@
         </is>
       </c>
       <c r="F32" s="1" t="n">
-        <v>542.758928</v>
+        <v>541.396936</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>543.478876</v>
-      </c>
-      <c r="H32" s="1" t="n">
-        <v>543.4028070000001</v>
-      </c>
+        <v>542.994313</v>
+      </c>
+      <c r="H32" s="1" t="n"/>
       <c r="I32" s="1" t="n">
-        <v>543.369931</v>
+        <v>542.753663</v>
       </c>
       <c r="J32" s="1" t="n">
-        <v>543.390173</v>
+        <v>542.828197</v>
       </c>
       <c r="K32" s="1" t="n">
-        <v>541.34</v>
+        <v>542.55</v>
       </c>
       <c r="L32" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[10], []]</t>
+          <t xml:space="preserve"> [[6], []]</t>
         </is>
       </c>
       <c r="M32" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 10]], []]</t>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
         </is>
       </c>
       <c r="N32" s="1" t="n">
-        <v>0.0164</v>
+        <v>0.0157</v>
       </c>
       <c r="O32" s="1" t="n">
-        <v>0.0274</v>
+        <v>0.0213</v>
       </c>
       <c r="P32" s="1" t="n">
-        <v>0.0219</v>
+        <v>0.0259</v>
       </c>
       <c r="Q32" s="1" t="n"/>
       <c r="R32" s="1" t="n"/>
@@ -2295,7 +2239,7 @@
     <row r="33">
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>co2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr">
@@ -2305,7 +2249,7 @@
       </c>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>STO-3G</t>
+          <t>4-31G</t>
         </is>
       </c>
       <c r="E33" s="1" t="inlineStr">
@@ -2314,41 +2258,41 @@
         </is>
       </c>
       <c r="F33" s="1" t="n">
-        <v>543.5513529999999</v>
+        <v>543.367484</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>544.308366</v>
+        <v>544.966489</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>544.031458</v>
+        <v>544.528882</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>544.020774</v>
+        <v>544.518913</v>
       </c>
       <c r="J33" s="1" t="n">
-        <v>544.334488</v>
+        <v>544.550709</v>
       </c>
       <c r="K33" s="1" t="n">
-        <v>541.34</v>
+        <v>542.55</v>
       </c>
       <c r="L33" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[10], []]</t>
+          <t xml:space="preserve"> [[6], []]</t>
         </is>
       </c>
       <c r="M33" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 10]], []]</t>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
         </is>
       </c>
       <c r="N33" s="1" t="n">
-        <v>0.0184</v>
+        <v>0.0177</v>
       </c>
       <c r="O33" s="1" t="n">
-        <v>0.0371</v>
+        <v>0.0258</v>
       </c>
       <c r="P33" s="1" t="n">
-        <v>0.0104</v>
+        <v>0.0287</v>
       </c>
       <c r="Q33" s="1" t="n"/>
       <c r="R33" s="1" t="n"/>
@@ -2357,7 +2301,7 @@
     <row r="34">
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>co2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr">
@@ -2367,7 +2311,7 @@
       </c>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>6-31G</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr">
@@ -2376,41 +2320,41 @@
         </is>
       </c>
       <c r="F34" s="1" t="n">
-        <v>541.713359</v>
+        <v>544.538315</v>
       </c>
       <c r="G34" s="1" t="n">
-        <v>543.164124</v>
+        <v>546.241719</v>
       </c>
       <c r="H34" s="1" t="n">
-        <v>543.148267</v>
+        <v>545.79014</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>543.112521</v>
+        <v>545.786166</v>
       </c>
       <c r="J34" s="1" t="n">
-        <v>543.137935</v>
+        <v>545.811799</v>
       </c>
       <c r="K34" s="1" t="n">
-        <v>541.34</v>
+        <v>542.55</v>
       </c>
       <c r="L34" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[10], []]</t>
+          <t xml:space="preserve"> [[6], []]</t>
         </is>
       </c>
       <c r="M34" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 10]], []]</t>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
         </is>
       </c>
       <c r="N34" s="1" t="n">
-        <v>0.0162</v>
+        <v>0.0179</v>
       </c>
       <c r="O34" s="1" t="n">
-        <v>0.0269</v>
+        <v>0.026</v>
       </c>
       <c r="P34" s="1" t="n">
-        <v>0.0217</v>
+        <v>0.0286</v>
       </c>
       <c r="Q34" s="1" t="n"/>
       <c r="R34" s="1" t="n"/>
@@ -2419,7 +2363,7 @@
     <row r="35">
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>co2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr">
@@ -2429,7 +2373,7 @@
       </c>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>ccX-DZ</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr">
@@ -2438,41 +2382,39 @@
         </is>
       </c>
       <c r="F35" s="1" t="n">
-        <v>540.403953</v>
+        <v>541.239409</v>
       </c>
       <c r="G35" s="1" t="n">
-        <v>541.4171720000001</v>
-      </c>
-      <c r="H35" s="1" t="n">
-        <v>541.464116</v>
-      </c>
+        <v>542.9506280000001</v>
+      </c>
+      <c r="H35" s="1" t="n"/>
       <c r="I35" s="1" t="n">
-        <v>541.397589</v>
+        <v>542.707344</v>
       </c>
       <c r="J35" s="1" t="n">
-        <v>541.454346</v>
+        <v>542.7963580000001</v>
       </c>
       <c r="K35" s="1" t="n">
-        <v>541.34</v>
+        <v>542.55</v>
       </c>
       <c r="L35" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[10], []]</t>
+          <t xml:space="preserve"> [[6], []]</t>
         </is>
       </c>
       <c r="M35" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 10]], []]</t>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
         </is>
       </c>
       <c r="N35" s="1" t="n">
-        <v>0.0152</v>
+        <v>0.0155</v>
       </c>
       <c r="O35" s="1" t="n">
-        <v>0.0261</v>
+        <v>0.0204</v>
       </c>
       <c r="P35" s="1" t="n">
-        <v>0.0203</v>
+        <v>0.0255</v>
       </c>
       <c r="Q35" s="1" t="n"/>
       <c r="R35" s="1" t="n"/>
@@ -2481,7 +2423,7 @@
     <row r="36">
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>co2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr">
@@ -2491,7 +2433,7 @@
       </c>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>def2svp</t>
         </is>
       </c>
       <c r="E36" s="1" t="inlineStr">
@@ -2500,33 +2442,1471 @@
         </is>
       </c>
       <c r="F36" s="1" t="n">
-        <v>540.383491</v>
+        <v>543.682769</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>541.405196</v>
-      </c>
-      <c r="H36" s="1" t="n"/>
-      <c r="I36" s="1" t="n"/>
-      <c r="J36" s="1" t="n"/>
+        <v>545.204682</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <v>544.834432</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>544.798126</v>
+      </c>
+      <c r="J36" s="1" t="n">
+        <v>544.868799</v>
+      </c>
       <c r="K36" s="1" t="n">
-        <v>541.34</v>
+        <v>542.55</v>
       </c>
       <c r="L36" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[10], []]</t>
+          <t xml:space="preserve"> [[6], []]</t>
         </is>
       </c>
       <c r="M36" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [[[0, 10]], []]</t>
-        </is>
-      </c>
-      <c r="N36" s="1" t="n"/>
-      <c r="O36" s="1" t="n"/>
-      <c r="P36" s="1" t="n"/>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
+        </is>
+      </c>
+      <c r="N36" s="1" t="n">
+        <v>0.0167</v>
+      </c>
+      <c r="O36" s="1" t="n">
+        <v>0.0234</v>
+      </c>
+      <c r="P36" s="1" t="n">
+        <v>0.0268</v>
+      </c>
       <c r="Q36" s="1" t="n"/>
       <c r="R36" s="1" t="n"/>
       <c r="S36" s="1" t="n"/>
+    </row>
+    <row r="37">
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>co</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D37" s="1" t="inlineStr">
+        <is>
+          <t>STO-3G</t>
+        </is>
+      </c>
+      <c r="E37" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>546.120439</v>
+      </c>
+      <c r="G37" s="1" t="n">
+        <v>548.022062</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <v>547.674501</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>547.5980070000001</v>
+      </c>
+      <c r="J37" s="1" t="n">
+        <v>547.669324</v>
+      </c>
+      <c r="K37" s="1" t="n">
+        <v>542.55</v>
+      </c>
+      <c r="L37" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[6], []]</t>
+        </is>
+      </c>
+      <c r="M37" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
+        </is>
+      </c>
+      <c r="N37" s="1" t="n">
+        <v>0.0176</v>
+      </c>
+      <c r="O37" s="1" t="n">
+        <v>0.0207</v>
+      </c>
+      <c r="P37" s="1" t="n">
+        <v>0.0194</v>
+      </c>
+      <c r="Q37" s="1" t="n"/>
+      <c r="R37" s="1" t="n"/>
+      <c r="S37" s="1" t="n"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>co</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D38" s="1" t="inlineStr">
+        <is>
+          <t>ccX-QZ</t>
+        </is>
+      </c>
+      <c r="E38" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>541.178795</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>542.892747</v>
+      </c>
+      <c r="H38" s="1" t="n"/>
+      <c r="I38" s="1" t="n">
+        <v>542.599076</v>
+      </c>
+      <c r="J38" s="1" t="n">
+        <v>542.719524</v>
+      </c>
+      <c r="K38" s="1" t="n">
+        <v>542.55</v>
+      </c>
+      <c r="L38" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[6], []]</t>
+        </is>
+      </c>
+      <c r="M38" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
+        </is>
+      </c>
+      <c r="N38" s="1" t="n">
+        <v>0.0152</v>
+      </c>
+      <c r="O38" s="1" t="n">
+        <v>0.0192</v>
+      </c>
+      <c r="P38" s="1" t="n">
+        <v>0.0246</v>
+      </c>
+      <c r="Q38" s="1" t="n"/>
+      <c r="R38" s="1" t="n"/>
+      <c r="S38" s="1" t="n"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>co</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D39" s="1" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E39" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>542.589644</v>
+      </c>
+      <c r="G39" s="1" t="n">
+        <v>544.813564</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <v>544.527342</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>544.4855209999999</v>
+      </c>
+      <c r="J39" s="1" t="n">
+        <v>544.557104</v>
+      </c>
+      <c r="K39" s="1" t="n">
+        <v>542.55</v>
+      </c>
+      <c r="L39" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[6], []]</t>
+        </is>
+      </c>
+      <c r="M39" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
+        </is>
+      </c>
+      <c r="N39" s="1" t="n">
+        <v>0.0162</v>
+      </c>
+      <c r="O39" s="1" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="P39" s="1" t="n">
+        <v>0.0267</v>
+      </c>
+      <c r="Q39" s="1" t="n"/>
+      <c r="R39" s="1" t="n"/>
+      <c r="S39" s="1" t="n"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>co</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D40" s="1" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="E40" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>541.207688</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>542.90394</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <v>542.675713</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>542.612129</v>
+      </c>
+      <c r="J40" s="1" t="n">
+        <v>542.7326880000001</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <v>542.55</v>
+      </c>
+      <c r="L40" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[6], []]</t>
+        </is>
+      </c>
+      <c r="M40" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
+        </is>
+      </c>
+      <c r="N40" s="1" t="n">
+        <v>0.0152</v>
+      </c>
+      <c r="O40" s="1" t="n">
+        <v>0.0192</v>
+      </c>
+      <c r="P40" s="1" t="n">
+        <v>0.0246</v>
+      </c>
+      <c r="Q40" s="1" t="n"/>
+      <c r="R40" s="1" t="n"/>
+      <c r="S40" s="1" t="n"/>
+    </row>
+    <row r="41">
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>co</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D41" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E41" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>541.181632</v>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>542.878792</v>
+      </c>
+      <c r="H41" s="1" t="n"/>
+      <c r="I41" s="1" t="n"/>
+      <c r="J41" s="1" t="n"/>
+      <c r="K41" s="1" t="n">
+        <v>542.55</v>
+      </c>
+      <c r="L41" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[6], []]</t>
+        </is>
+      </c>
+      <c r="M41" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 6]], []]</t>
+        </is>
+      </c>
+      <c r="N41" s="1" t="n"/>
+      <c r="O41" s="1" t="n"/>
+      <c r="P41" s="1" t="n"/>
+      <c r="Q41" s="1" t="n"/>
+      <c r="R41" s="1" t="n"/>
+      <c r="S41" s="1" t="n"/>
+    </row>
+    <row r="42">
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D42" s="1" t="inlineStr">
+        <is>
+          <t>pcX-2</t>
+        </is>
+      </c>
+      <c r="E42" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>540.405314</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>541.374544</v>
+      </c>
+      <c r="H42" s="1" t="n"/>
+      <c r="I42" s="1" t="n">
+        <v>541.368218</v>
+      </c>
+      <c r="J42" s="1" t="n">
+        <v>541.417065</v>
+      </c>
+      <c r="K42" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L42" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M42" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N42" s="1" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="O42" s="1" t="n">
+        <v>0.0265</v>
+      </c>
+      <c r="P42" s="1" t="n">
+        <v>0.0206</v>
+      </c>
+      <c r="Q42" s="1" t="n"/>
+      <c r="R42" s="1" t="n"/>
+      <c r="S42" s="1" t="n"/>
+    </row>
+    <row r="43">
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D43" s="1" t="inlineStr">
+        <is>
+          <t>def2svpd</t>
+        </is>
+      </c>
+      <c r="E43" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>542.840658</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>543.7178730000001</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>543.622133</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>543.587229</v>
+      </c>
+      <c r="J43" s="1" t="n">
+        <v>543.64082</v>
+      </c>
+      <c r="K43" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L43" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M43" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N43" s="1" t="n">
+        <v>0.0162</v>
+      </c>
+      <c r="O43" s="1" t="n">
+        <v>0.0272</v>
+      </c>
+      <c r="P43" s="1" t="n">
+        <v>0.0218</v>
+      </c>
+      <c r="Q43" s="1" t="n"/>
+      <c r="R43" s="1" t="n"/>
+      <c r="S43" s="1" t="n"/>
+    </row>
+    <row r="44">
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D44" s="1" t="inlineStr">
+        <is>
+          <t>pcX-4</t>
+        </is>
+      </c>
+      <c r="E44" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>552.284586</v>
+      </c>
+      <c r="G44" s="1" t="n">
+        <v>553.2306</v>
+      </c>
+      <c r="H44" s="1" t="n"/>
+      <c r="I44" s="1" t="n"/>
+      <c r="J44" s="1" t="n"/>
+      <c r="K44" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L44" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M44" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N44" s="1" t="n"/>
+      <c r="O44" s="1" t="n"/>
+      <c r="P44" s="1" t="n"/>
+      <c r="Q44" s="1" t="n"/>
+      <c r="R44" s="1" t="n"/>
+      <c r="S44" s="1" t="n"/>
+    </row>
+    <row r="45">
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D45" s="1" t="inlineStr">
+        <is>
+          <t>pcX-3</t>
+        </is>
+      </c>
+      <c r="E45" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>540.384141</v>
+      </c>
+      <c r="G45" s="1" t="n">
+        <v>541.344009</v>
+      </c>
+      <c r="H45" s="1" t="n"/>
+      <c r="I45" s="1" t="n">
+        <v>541.3237</v>
+      </c>
+      <c r="J45" s="1" t="n">
+        <v>541.38312</v>
+      </c>
+      <c r="K45" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L45" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M45" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N45" s="1" t="n">
+        <v>0.0153</v>
+      </c>
+      <c r="O45" s="1" t="n">
+        <v>0.0263</v>
+      </c>
+      <c r="P45" s="1" t="n">
+        <v>0.0205</v>
+      </c>
+      <c r="Q45" s="1" t="n"/>
+      <c r="R45" s="1" t="n"/>
+      <c r="S45" s="1" t="n"/>
+    </row>
+    <row r="46">
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D46" s="1" t="inlineStr">
+        <is>
+          <t>3-21G</t>
+        </is>
+      </c>
+      <c r="E46" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>540.712431</v>
+      </c>
+      <c r="G46" s="1" t="n">
+        <v>540.817708</v>
+      </c>
+      <c r="H46" s="1" t="n">
+        <v>540.803845</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>540.76192</v>
+      </c>
+      <c r="J46" s="1" t="n">
+        <v>540.820592</v>
+      </c>
+      <c r="K46" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L46" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M46" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N46" s="1" t="n">
+        <v>0.0173</v>
+      </c>
+      <c r="O46" s="1" t="n">
+        <v>0.0303</v>
+      </c>
+      <c r="P46" s="1" t="n">
+        <v>0.0201</v>
+      </c>
+      <c r="Q46" s="1" t="n"/>
+      <c r="R46" s="1" t="n"/>
+      <c r="S46" s="1" t="n"/>
+    </row>
+    <row r="47">
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D47" s="1" t="inlineStr">
+        <is>
+          <t>STO-6G</t>
+        </is>
+      </c>
+      <c r="E47" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>550.647015</v>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>551.428781</v>
+      </c>
+      <c r="H47" s="1" t="n">
+        <v>551.142123</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>551.1091300000001</v>
+      </c>
+      <c r="J47" s="1" t="n">
+        <v>551.429568</v>
+      </c>
+      <c r="K47" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L47" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M47" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N47" s="1" t="n">
+        <v>0.0187</v>
+      </c>
+      <c r="O47" s="1" t="n">
+        <v>0.0417</v>
+      </c>
+      <c r="P47" s="1" t="n">
+        <v>0.0103</v>
+      </c>
+      <c r="Q47" s="1" t="n"/>
+      <c r="R47" s="1" t="n"/>
+      <c r="S47" s="1" t="n"/>
+    </row>
+    <row r="48">
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D48" s="1" t="inlineStr">
+        <is>
+          <t>ccX-TZ</t>
+        </is>
+      </c>
+      <c r="E48" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>540.387932</v>
+      </c>
+      <c r="G48" s="1" t="n">
+        <v>541.438358</v>
+      </c>
+      <c r="H48" s="1" t="n"/>
+      <c r="I48" s="1" t="n">
+        <v>541.426778</v>
+      </c>
+      <c r="J48" s="1" t="n">
+        <v>541.4775100000001</v>
+      </c>
+      <c r="K48" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L48" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M48" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N48" s="1" t="n">
+        <v>0.0153</v>
+      </c>
+      <c r="O48" s="1" t="n">
+        <v>0.0262</v>
+      </c>
+      <c r="P48" s="1" t="n">
+        <v>0.0205</v>
+      </c>
+      <c r="Q48" s="1" t="n"/>
+      <c r="R48" s="1" t="n"/>
+      <c r="S48" s="1" t="n"/>
+    </row>
+    <row r="49">
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D49" s="1" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E49" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>540.50555</v>
+      </c>
+      <c r="G49" s="1" t="n">
+        <v>541.48218</v>
+      </c>
+      <c r="H49" s="1" t="n">
+        <v>541.539387</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <v>541.475468</v>
+      </c>
+      <c r="J49" s="1" t="n">
+        <v>541.526035</v>
+      </c>
+      <c r="K49" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L49" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M49" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N49" s="1" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="O49" s="1" t="n">
+        <v>0.0262</v>
+      </c>
+      <c r="P49" s="1" t="n">
+        <v>0.0206</v>
+      </c>
+      <c r="Q49" s="1" t="n"/>
+      <c r="R49" s="1" t="n"/>
+      <c r="S49" s="1" t="n"/>
+    </row>
+    <row r="50">
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D50" s="1" t="inlineStr">
+        <is>
+          <t>ccX-5Z</t>
+        </is>
+      </c>
+      <c r="E50" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>540.382309</v>
+      </c>
+      <c r="G50" s="1" t="n">
+        <v>541.413899</v>
+      </c>
+      <c r="H50" s="1" t="n"/>
+      <c r="I50" s="1" t="n"/>
+      <c r="J50" s="1" t="n"/>
+      <c r="K50" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L50" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M50" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N50" s="1" t="n"/>
+      <c r="O50" s="1" t="n"/>
+      <c r="P50" s="1" t="n"/>
+      <c r="Q50" s="1" t="n"/>
+      <c r="R50" s="1" t="n"/>
+      <c r="S50" s="1" t="n"/>
+    </row>
+    <row r="51">
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D51" s="1" t="inlineStr">
+        <is>
+          <t>pcX-1</t>
+        </is>
+      </c>
+      <c r="E51" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>540.6099</v>
+      </c>
+      <c r="G51" s="1" t="n">
+        <v>541.47535</v>
+      </c>
+      <c r="H51" s="1" t="n"/>
+      <c r="I51" s="1" t="n">
+        <v>541.518904</v>
+      </c>
+      <c r="J51" s="1" t="n">
+        <v>541.53653</v>
+      </c>
+      <c r="K51" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L51" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M51" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N51" s="1" t="n">
+        <v>0.0157</v>
+      </c>
+      <c r="O51" s="1" t="n">
+        <v>0.0266</v>
+      </c>
+      <c r="P51" s="1" t="n">
+        <v>0.0211</v>
+      </c>
+      <c r="Q51" s="1" t="n"/>
+      <c r="R51" s="1" t="n"/>
+      <c r="S51" s="1" t="n"/>
+    </row>
+    <row r="52">
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D52" s="1" t="inlineStr">
+        <is>
+          <t>4-31G</t>
+        </is>
+      </c>
+      <c r="E52" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>542.634949</v>
+      </c>
+      <c r="G52" s="1" t="n">
+        <v>543.299207</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <v>543.241</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <v>543.20036</v>
+      </c>
+      <c r="J52" s="1" t="n">
+        <v>543.227394</v>
+      </c>
+      <c r="K52" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L52" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M52" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N52" s="1" t="n">
+        <v>0.0172</v>
+      </c>
+      <c r="O52" s="1" t="n">
+        <v>0.0326</v>
+      </c>
+      <c r="P52" s="1" t="n">
+        <v>0.0206</v>
+      </c>
+      <c r="Q52" s="1" t="n"/>
+      <c r="R52" s="1" t="n"/>
+      <c r="S52" s="1" t="n"/>
+    </row>
+    <row r="53">
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D53" s="1" t="inlineStr">
+        <is>
+          <t>6-31G</t>
+        </is>
+      </c>
+      <c r="E53" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>543.774725</v>
+      </c>
+      <c r="G53" s="1" t="n">
+        <v>544.53587</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <v>544.465741</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <v>544.4301390000001</v>
+      </c>
+      <c r="J53" s="1" t="n">
+        <v>544.45589</v>
+      </c>
+      <c r="K53" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L53" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M53" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N53" s="1" t="n">
+        <v>0.0171</v>
+      </c>
+      <c r="O53" s="1" t="n">
+        <v>0.0325</v>
+      </c>
+      <c r="P53" s="1" t="n">
+        <v>0.0205</v>
+      </c>
+      <c r="Q53" s="1" t="n"/>
+      <c r="R53" s="1" t="n"/>
+      <c r="S53" s="1" t="n"/>
+    </row>
+    <row r="54">
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D54" s="1" t="inlineStr">
+        <is>
+          <t>ccX-DZ</t>
+        </is>
+      </c>
+      <c r="E54" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>540.433371</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <v>541.451124</v>
+      </c>
+      <c r="H54" s="1" t="n"/>
+      <c r="I54" s="1" t="n">
+        <v>541.464581</v>
+      </c>
+      <c r="J54" s="1" t="n">
+        <v>541.506001</v>
+      </c>
+      <c r="K54" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L54" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M54" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N54" s="1" t="n">
+        <v>0.0155</v>
+      </c>
+      <c r="O54" s="1" t="n">
+        <v>0.0267</v>
+      </c>
+      <c r="P54" s="1" t="n">
+        <v>0.0205</v>
+      </c>
+      <c r="Q54" s="1" t="n"/>
+      <c r="R54" s="1" t="n"/>
+      <c r="S54" s="1" t="n"/>
+    </row>
+    <row r="55">
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D55" s="1" t="inlineStr">
+        <is>
+          <t>def2svp</t>
+        </is>
+      </c>
+      <c r="E55" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>542.758928</v>
+      </c>
+      <c r="G55" s="1" t="n">
+        <v>543.478876</v>
+      </c>
+      <c r="H55" s="1" t="n">
+        <v>543.4028070000001</v>
+      </c>
+      <c r="I55" s="1" t="n">
+        <v>543.369931</v>
+      </c>
+      <c r="J55" s="1" t="n">
+        <v>543.390173</v>
+      </c>
+      <c r="K55" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L55" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M55" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N55" s="1" t="n">
+        <v>0.0164</v>
+      </c>
+      <c r="O55" s="1" t="n">
+        <v>0.0274</v>
+      </c>
+      <c r="P55" s="1" t="n">
+        <v>0.0219</v>
+      </c>
+      <c r="Q55" s="1" t="n"/>
+      <c r="R55" s="1" t="n"/>
+      <c r="S55" s="1" t="n"/>
+    </row>
+    <row r="56">
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D56" s="1" t="inlineStr">
+        <is>
+          <t>STO-3G</t>
+        </is>
+      </c>
+      <c r="E56" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>543.5513529999999</v>
+      </c>
+      <c r="G56" s="1" t="n">
+        <v>544.308366</v>
+      </c>
+      <c r="H56" s="1" t="n">
+        <v>544.031458</v>
+      </c>
+      <c r="I56" s="1" t="n">
+        <v>544.020774</v>
+      </c>
+      <c r="J56" s="1" t="n">
+        <v>544.334488</v>
+      </c>
+      <c r="K56" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L56" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M56" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N56" s="1" t="n">
+        <v>0.0184</v>
+      </c>
+      <c r="O56" s="1" t="n">
+        <v>0.0371</v>
+      </c>
+      <c r="P56" s="1" t="n">
+        <v>0.0104</v>
+      </c>
+      <c r="Q56" s="1" t="n"/>
+      <c r="R56" s="1" t="n"/>
+      <c r="S56" s="1" t="n"/>
+    </row>
+    <row r="57">
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D57" s="1" t="inlineStr">
+        <is>
+          <t>ccX-QZ</t>
+        </is>
+      </c>
+      <c r="E57" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F57" s="1" t="n">
+        <v>540.382734</v>
+      </c>
+      <c r="G57" s="1" t="n">
+        <v>541.419829</v>
+      </c>
+      <c r="H57" s="1" t="n"/>
+      <c r="I57" s="1" t="n">
+        <v>541.39613</v>
+      </c>
+      <c r="J57" s="1" t="n">
+        <v>541.4534</v>
+      </c>
+      <c r="K57" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L57" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M57" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N57" s="1" t="n">
+        <v>0.0152</v>
+      </c>
+      <c r="O57" s="1" t="n">
+        <v>0.0261</v>
+      </c>
+      <c r="P57" s="1" t="n">
+        <v>0.0203</v>
+      </c>
+      <c r="Q57" s="1" t="n"/>
+      <c r="R57" s="1" t="n"/>
+      <c r="S57" s="1" t="n"/>
+    </row>
+    <row r="58">
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D58" s="1" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E58" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F58" s="1" t="n">
+        <v>541.713359</v>
+      </c>
+      <c r="G58" s="1" t="n">
+        <v>543.164124</v>
+      </c>
+      <c r="H58" s="1" t="n">
+        <v>543.148267</v>
+      </c>
+      <c r="I58" s="1" t="n">
+        <v>543.112521</v>
+      </c>
+      <c r="J58" s="1" t="n">
+        <v>543.137935</v>
+      </c>
+      <c r="K58" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L58" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M58" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N58" s="1" t="n">
+        <v>0.0162</v>
+      </c>
+      <c r="O58" s="1" t="n">
+        <v>0.0269</v>
+      </c>
+      <c r="P58" s="1" t="n">
+        <v>0.0217</v>
+      </c>
+      <c r="Q58" s="1" t="n"/>
+      <c r="R58" s="1" t="n"/>
+      <c r="S58" s="1" t="n"/>
+    </row>
+    <row r="59">
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D59" s="1" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="E59" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F59" s="1" t="n">
+        <v>540.403953</v>
+      </c>
+      <c r="G59" s="1" t="n">
+        <v>541.4171720000001</v>
+      </c>
+      <c r="H59" s="1" t="n">
+        <v>541.464116</v>
+      </c>
+      <c r="I59" s="1" t="n">
+        <v>541.397589</v>
+      </c>
+      <c r="J59" s="1" t="n">
+        <v>541.454346</v>
+      </c>
+      <c r="K59" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L59" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M59" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N59" s="1" t="n">
+        <v>0.0152</v>
+      </c>
+      <c r="O59" s="1" t="n">
+        <v>0.0261</v>
+      </c>
+      <c r="P59" s="1" t="n">
+        <v>0.0203</v>
+      </c>
+      <c r="Q59" s="1" t="n"/>
+      <c r="R59" s="1" t="n"/>
+      <c r="S59" s="1" t="n"/>
+    </row>
+    <row r="60">
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>co2</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D60" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E60" s="1" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F60" s="1" t="n">
+        <v>540.383491</v>
+      </c>
+      <c r="G60" s="1" t="n">
+        <v>541.405196</v>
+      </c>
+      <c r="H60" s="1" t="n"/>
+      <c r="I60" s="1" t="n"/>
+      <c r="J60" s="1" t="n"/>
+      <c r="K60" s="1" t="n">
+        <v>541.34</v>
+      </c>
+      <c r="L60" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[10], []]</t>
+        </is>
+      </c>
+      <c r="M60" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [[[0, 10]], []]</t>
+        </is>
+      </c>
+      <c r="N60" s="1" t="n"/>
+      <c r="O60" s="1" t="n"/>
+      <c r="P60" s="1" t="n"/>
+      <c r="Q60" s="1" t="n"/>
+      <c r="R60" s="1" t="n"/>
+      <c r="S60" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>